<commit_message>
Fixing aprox graphs limits
</commit_message>
<xml_diff>
--- a/projeto1/test/graphs/xls/aprox-error-1-100MB.xlsx
+++ b/projeto1/test/graphs/xls/aprox-error-1-100MB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betoc\Documents\graphs\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betoc\Documents\git\string-processing\projeto1\test\graphs\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -765,52 +765,141 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="24"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>13</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>17</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>18</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>19</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>21</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>22</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>23</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>24</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v>25</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'result-aprox-error-1-50MB'!$E$1:$E$15</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'result-aprox-error-1-50MB'!$E$1:$E$15</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'result-aprox-error-1-50MB'!$E$2:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.71899999999999997</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71899999999999997</c:v>
+                  <c:v>0.83699999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83699999999999997</c:v>
+                  <c:v>0.84199999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84199999999999997</c:v>
+                  <c:v>0.69099999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.69099999999999995</c:v>
+                  <c:v>1.139</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.139</c:v>
+                  <c:v>0.751</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.751</c:v>
+                  <c:v>0.68300000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68300000000000005</c:v>
+                  <c:v>1.115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.115</c:v>
+                  <c:v>1.113</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.113</c:v>
+                  <c:v>0.68600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.68600000000000005</c:v>
+                  <c:v>0.68400000000000005</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.68400000000000005</c:v>
+                  <c:v>0.68200000000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.68200000000000005</c:v>
+                  <c:v>0.72099999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.72099999999999997</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>0.68400000000000005</c:v>
                 </c:pt>
               </c:numCache>
@@ -861,82 +950,171 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="24"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>13</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>17</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>18</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>19</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>21</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>22</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>23</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>24</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v>25</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'result-aprox-error-1-50MB'!$E$16:$E$40</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'result-aprox-error-1-50MB'!$E$16:$E$40</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'result-aprox-error-1-50MB'!$E$17:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1.542</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.542</c:v>
+                  <c:v>1.8029999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8029999999999999</c:v>
+                  <c:v>1.7869999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7869999999999999</c:v>
+                  <c:v>2.052</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.052</c:v>
+                  <c:v>2.1890000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1890000000000001</c:v>
+                  <c:v>2.5099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5099999999999998</c:v>
+                  <c:v>2.9489999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9489999999999998</c:v>
+                  <c:v>3.1960000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.1960000000000002</c:v>
+                  <c:v>3.323</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.323</c:v>
+                  <c:v>3.59</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.59</c:v>
+                  <c:v>4.0010000000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.0010000000000003</c:v>
+                  <c:v>4.3719999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.3719999999999999</c:v>
+                  <c:v>4.6360000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.6360000000000001</c:v>
+                  <c:v>4.17</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.17</c:v>
+                  <c:v>5.3769999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.3769999999999998</c:v>
+                  <c:v>5.3440000000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.3440000000000003</c:v>
+                  <c:v>5.6689999999999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.6689999999999996</c:v>
+                  <c:v>6.2210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.2210000000000001</c:v>
+                  <c:v>6.8630000000000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.8630000000000004</c:v>
+                  <c:v>7.06</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.06</c:v>
+                  <c:v>7.6349999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.6349999999999998</c:v>
+                  <c:v>7.4390000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.4390000000000001</c:v>
+                  <c:v>7.74</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.74</c:v>
-                </c:pt>
-                <c:pt idx="24">
                   <c:v>8.1519999999999992</c:v>
                 </c:pt>
               </c:numCache>
@@ -987,82 +1165,171 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="24"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>13</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>17</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>18</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>19</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>21</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>22</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>23</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>24</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v>25</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'result-aprox-error-1-50MB'!$E$41:$E$65</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'result-aprox-error-1-50MB'!$E$41:$E$65</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'result-aprox-error-1-50MB'!$E$42:$E$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>0.91900000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91900000000000004</c:v>
+                  <c:v>0.71499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71499999999999997</c:v>
+                  <c:v>0.67800000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67800000000000005</c:v>
+                  <c:v>0.68300000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.68300000000000005</c:v>
+                  <c:v>0.68200000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.69599999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.70599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.70599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.68200000000000005</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.69599999999999995</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.70599999999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.70699999999999996</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.70599999999999996</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.68200000000000005</c:v>
+                  <c:v>0.69299999999999995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.69299999999999995</c:v>
+                  <c:v>0.67700000000000005</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.67700000000000005</c:v>
+                  <c:v>0.67300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.67300000000000004</c:v>
+                  <c:v>0.69799999999999995</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.69799999999999995</c:v>
+                  <c:v>0.71599999999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.71599999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.71599999999999997</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.77</c:v>
+                  <c:v>0.71899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.71899999999999997</c:v>
+                  <c:v>0.69799999999999995</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.69799999999999995</c:v>
+                  <c:v>0.73399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.73399999999999999</c:v>
+                  <c:v>0.76900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.76900000000000002</c:v>
+                  <c:v>0.70799999999999996</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.70799999999999996</c:v>
-                </c:pt>
-                <c:pt idx="24">
                   <c:v>0.72799999999999998</c:v>
                 </c:pt>
               </c:numCache>

</xml_diff>